<commit_message>
Maximiza tela no selenium e ajustes no requeriments
</commit_message>
<xml_diff>
--- a/Ofertas.xlsx
+++ b/Ofertas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.lebiscuit.com.br/iphone-12-apple-64gb-tela-de-6-1-polegadas-camera-12mp-ios-16597al08l832478/p%3Fidsku%3D2147376583&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQgOUECMkO&amp;usg=AOvVaw2cFoiuHfIiQ-0tBcdnXtoN</t>
+          <t>https://www.google.com/url?url=https://www.lebiscuit.com.br/iphone-12-apple-64gb-tela-de-6-1-polegadas-camera-12mp-ios-16597al08l832478/p%3Fidsku%3D2147376583&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQgOUECP8N&amp;usg=AOvVaw1sxxN35YJdbbmagNBLXr-S</t>
         </is>
       </c>
     </row>
@@ -472,41 +472,41 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3299</v>
+        <v>3379</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.trocafone.com.br/iphone-12-64gb-azul---excelente-70613/p%3Fidsku%3D39869&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQguUECPQP&amp;usg=AOvVaw3sY2Lj90OPMYRIk5CZmB2M</t>
+          <t>https://www.google.com/url?url=https://www.trocafone.com.br/iphone-12-64gb-azul---excelente-70613/p%3Fidsku%3D39869&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQguUECKoP&amp;usg=AOvVaw0YyKGqD3oITCUweNcmrHnF</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>usado: iphone 12 64gb preto - excelente</t>
+          <t>usado: iphone 12 64gb vermelho excelente - trocafone</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3089</v>
+        <v>3209</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.cea.com.br/usado--iphone-12-64gb-preto---excelente-4256307/p%3FskuId%3D5684085%26srsltid%3DAfmBOoqnVzmQhj3bQtKf778t700qZc21R9Lb4PCj1AIKCqq72sL7sZZ3XF0&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQgOUECKMQ&amp;usg=AOvVaw0_VCc7fhvPfdJJ3FWBSjrL</t>
+          <t>https://www.google.com/url?url=%23&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQgOUECOwP&amp;usg=AOvVaw0ELP03YRLky63eVe8qMhUy</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>iphone 12 64gb preto, super conservado! | celular iphone | usado</t>
+          <t>usado: iphone 12 64gb branco excelente - trocafone</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3454</v>
+        <v>3209</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-preto-super-conservado-92855609%3Fg_campaign%3Dgoogle_shopping%26srsltid%3DAfmBOooNrHXt0q-z4q8oSqyE6NaZ2tC0sVMmgoge5dRO0tAgk66pgQbsOew&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQgOUECI4R&amp;usg=AOvVaw0_jAM3itKktktXnZcQgMqc</t>
+          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/usado-iphone-12-64gb-branco-excelente-trocafone-1561610772/p/1561610772%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1561610772%26idLojista%3D33013%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQgOUECOoQ&amp;usg=AOvVaw2JaTFQyj-bFxPV3GFIdaaY</t>
         </is>
       </c>
     </row>
@@ -521,22 +521,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-preto-64gb-mp929837648/p&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQgOUECK8S&amp;usg=AOvVaw1M_yvWgTVGzf2WyuAHdvZ1</t>
+          <t>https://www.google.com/url?url=https://www.carrefour.com.br/vitrine-iphone-12-preto-64gb-mp929837648/p&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQgOUECLoR&amp;usg=AOvVaw2kPrazmE3tzY-rx2dyp3FC</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>iphone 12 intacto 64gb | celular apple | usado</t>
+          <t>iphone 12 64gb | celular apple | usado</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3415</v>
+        <v>3315</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-intacto-64gb-86967057%3Fg_campaign%3Dgoogle_shopping%26srsltid%3DAfmBOornP3gJrS6XVg7WLTSLBTOtpd-91fGj6KsjUKjIcF5qmwl9d6GF4hk&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjDuuK8vc-CAxWeGLkGHeZECsEQgOUECJET&amp;usg=AOvVaw2gLLmpAaO5oPQi_3QcEA1l</t>
+          <t>https://www.google.com/url?url=https://www.enjoei.com.br/p/iphone-12-64gb-93394889%3Fg_campaign%3Dgoogle_shopping%26srsltid%3DAfmBOortXtLZvDOqq1sItyjrGQONVn_Qk310LKRAjzTsuSMcG2VLECaWKEo&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjK69Gf5tWCAxXeALkGHSUvAroQgOUECMoR&amp;usg=AOvVaw2UmlbIqLpkQKm1KLx94GKM</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://gamernareal.com.br/product/placa-de-video-msi-geforce-rtx-2060-ventus-gp/%3Futm_source%3DGoogle%2520Shopping%26utm_campaign%3DGoogle%2520Menor%2520Preco%26utm_medium%3Dcpc%26utm_term%3D7362&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwip273Dvc-CAxW0LrkGHcYFBKkQguUECIoM&amp;usg=AOvVaw0XXT7fdCElpCHt30kKMA6X</t>
+          <t>https://www.google.com/url?url=https://gamernareal.com.br/product/placa-de-video-msi-geforce-rtx-2060-ventus-gp/%3Futm_source%3DGoogle%2520Shopping%26utm_campaign%3DGoogle%2520Menor%2520Preco%26utm_medium%3Dcpc%26utm_term%3D7362&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwin_Mum5tWCAxX3HrkGHYMVCmkQguUECJkL&amp;usg=AOvVaw3OOqLcTtPly5vSBRB_ItCU</t>
         </is>
       </c>
     </row>
@@ -581,82 +581,67 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/placa-video-pcwinmax-nvidia-geforce-rtx-2060-12gb-192bits-1559067608/p/1559067608%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1559067608%26idLojista%3D12231%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwip273Dvc-CAxW0LrkGHcYFBKkQguUECMQN&amp;usg=AOvVaw3mxNGA8M7iS8CmefKA00zf</t>
+          <t>https://www.google.com/url?url=https://www.casasbahia.com.br/placa-video-pcwinmax-nvidia-geforce-rtx-2060-12gb-192bits-1559067608/p/1559067608%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1559067608%26idLojista%3D12231%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwin_Mum5tWCAxX3HrkGHYMVCmkQguUECOwM&amp;usg=AOvVaw0eEqjWpPnNQi9mQBYTDd3P</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>placa de vídeo pci exp. 8gb/256bits rtx2060 super golden memory rtx2060-8gd6 ...</t>
+          <t>placa de vídeo pcyes geforce rtx 2060 6gb gddr6 192 bits</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2160.39</v>
+        <v>2199</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.gpj.com.br/produto/vga-pci-exp-8gb256bits-rtx2060-super-golden-memory-rtx2060-8gd6-gddr6-box&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwip273Dvc-CAxW0LrkGHcYFBKkQgOUECNoR&amp;usg=AOvVaw0osdGKFbWduj1IHoXAfIgH</t>
+          <t>https://www.google.com/url?url=https://www.fujioka.com.br/placa-de-video-pcyes-nvidia-geforce-rtx-2060-6gb-gddr6-192-bits-dual-fan-pax2060rtx6g192bdf-801221/p%3Fidsku%3D27526&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwin_Mum5tWCAxX3HrkGHYMVCmkQguUECPwN&amp;usg=AOvVaw1U7jE4_D3InWomTlfOLbds</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>placa de video colorful geforce rtx 2060 super nb v2-v 8gb gddr6 256bi</t>
+          <t>nova placa de vídeo asus dual geforce rtx 2060 evo oc edition 12gddr6 gb memória</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2022.15</v>
+        <v>2028.16</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.kabum.com.br/produto/387961/placa-de-video-colorful-nvidia-geforce-rtx-2060-super-nb-v2-v-8gb-gddr6-256-bits%3Fsrsltid%3DAfmBOoorEhyovn4Tzy3Y19dFtRBwwfwuRfD7sNKrDplrtkdySjP81xYdpbM&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwip273Dvc-CAxW0LrkGHcYFBKkQguUECI4S&amp;usg=AOvVaw1ZVAJKmR-a9PgV7_aZvEus</t>
+          <t>https://www.google.com/url?url=https://www.ebay.com/itm/255821325545%3Fchn%3Dps%26mkevt%3D1%26mkcid%3D28&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwin_Mum5tWCAxX3HrkGHYMVCmkQgOUECMwO&amp;usg=AOvVaw1cO4NyHqVsERmt2qAF0R2H</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>placa de vídeo evga nvidia geforce rtx 2060 ko ultra gaming</t>
+          <t>evga placa de vídeo nvidia geforce rtx 2060 6gb gddr6</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2238.99</v>
+        <v>1990</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?url=https://www.lognetinfo.com.br/produto%3FidProduto%3Dplaca-de-video-evga-rtx-2060-ko-ultra-gaming-nvidia-geforce-6gb-gddr6-192bit-dp-dvi-hdmi-06g-p4-2068-kr&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwip273Dvc-CAxW0LrkGHcYFBKkQguUECLAS&amp;usg=AOvVaw2JKf6cKbPQGjJAQkpN4EMG</t>
+          <t>https://www.buscape.com.br/lead?oid=1139015123&amp;channel=86&amp;index=2&amp;searchterm=rtx%202060</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>evga placa de vídeo nvidia geforce rtx 2060 6gb gddr6</t>
+          <t>evga placa gráfica geforce rtx 2060 sc gaming, 6gb gddr6, hdb fan 06g-p4-2062-kr</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1990</v>
+        <v>1979.9</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.buscape.com.br/lead?oid=1139015123&amp;channel=86&amp;index=3&amp;searchterm=rtx%202060</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>evga placa gráfica geforce rtx 2060 sc gaming, 6gb gddr6, hdb fan 06g-p4-2062-kr</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2148.2</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>https://www.buscape.com.br/lead?oid=841411028&amp;channel=86&amp;index=9&amp;searchterm=rtx%202060</t>
+          <t>https://www.buscape.com.br/lead?oid=841411028&amp;channel=86&amp;index=3&amp;searchterm=rtx%202060</t>
         </is>
       </c>
     </row>

</xml_diff>